<commit_message>
moving frames in folder corresponding to class
</commit_message>
<xml_diff>
--- a/data/multicam.xlsx
+++ b/data/multicam.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/Desktop/open_fall_detector/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57BFB839-A6F4-DA48-8EA4-9CD616294275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D845FE66-5097-2643-946C-5BEFAC356C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="17180" activeTab="1" xr2:uid="{C2E1A4E4-0957-A64E-B875-472D8B6EEEBE}"/>
+    <workbookView xWindow="1100" yWindow="660" windowWidth="27540" windowHeight="17180" activeTab="2" xr2:uid="{C2E1A4E4-0957-A64E-B875-472D8B6EEEBE}"/>
   </bookViews>
   <sheets>
     <sheet name="delay_frames" sheetId="1" r:id="rId1"/>
     <sheet name="labels" sheetId="2" r:id="rId2"/>
+    <sheet name="classes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>camera_1</t>
   </si>
@@ -74,6 +75,33 @@
   </si>
   <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>falling</t>
+  </si>
+  <si>
+    <t>lying_on_the_ground</t>
+  </si>
+  <si>
+    <t>crounching</t>
+  </si>
+  <si>
+    <t>moving_down</t>
+  </si>
+  <si>
+    <t>moving_up</t>
+  </si>
+  <si>
+    <t>sitting</t>
+  </si>
+  <si>
+    <t>lying_on_a_sofa</t>
+  </si>
+  <si>
+    <t>moving_horizontaly</t>
+  </si>
+  <si>
+    <t>walking_or_standing_up</t>
   </si>
 </sst>
 </file>
@@ -428,7 +456,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269CC0B2-A610-3D4D-88B6-621C5957EA10}">
   <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3976,4 +4004,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EDFC70-9706-6B40-9B0C-BB3BDFB9F87A}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="243" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>